<commit_message>
most of the chapter 1 fixes/revisions.
</commit_message>
<xml_diff>
--- a/chapters/ch01-Introduction/datasets/exponential.xlsx
+++ b/chapters/ch01-Introduction/datasets/exponential.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://calvincollege-my.sharepoint.com/personal/jva_calvin_edu/Documents/Documents/latex/books/MCBook2021/chapters/ch01-Introduction/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{69472355-1805-4240-9C9D-DD54CCCD29E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1721F68-F6E1-466C-8DE3-9FF63C5B5BCD}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{69472355-1805-4240-9C9D-DD54CCCD29E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0804F122-35FA-4C15-B40A-80A08BDD4618}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{483FBEEC-619D-494D-A178-63EB4F9C2C50}"/>
   </bookViews>
@@ -1342,8 +1342,1145 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>B</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$370</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="369"/>
+                <c:pt idx="0">
+                  <c:v>1.0100501670841679</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0202013400267558</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0304545339535169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0408107741923882</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0512710963760241</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0618365465453596</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0725081812542165</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0832870676749586</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0941742837052104</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1051709180756477</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1162780704588713</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1274968515793757</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1388283833246218</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1502737988572274</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1618342427282831</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.1735108709918103</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.1853048513203654</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1972173631218102</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2092495976572515</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2214027581601699</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2336780599567432</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2460767305873808</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2586000099294778</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2712491503214047</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2840254166877414</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.2969300866657718</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.3099644507332473</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.3231298123374369</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.3364274880254721</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.3498588075760032</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.3634251141321778</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.3771277643359572</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.3909681284637803</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.4049475905635938</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.4190675485932571</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.4333294145603401</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.4477346146633245</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.4622845894342245</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.4769807938826427</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4918246976412703</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.5068177851128535</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.5219615556186337</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.5372575235482815</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.552707218511336</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.5683121854901689</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.5840739849944818</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.5999941932173602</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.6160744021928934</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.6323162199553789</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.6487212707001282</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.6652911949458864</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.6820276496988864</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.6989323086185506</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.7160068621848585</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.7332530178673953</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.7506725002961012</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.7682670514337351</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.7860384307500734</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.8039884153978569</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.8221188003905089</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.8404313987816374</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.8589280418463421</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.8776105792643432</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.8964808793049515</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.9155408290138962</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.9347923344020317</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.9542373206359396</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.9738777322304477</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.9937155332430823</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>2.0137527074704766</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>2.0339912586467506</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>2.0544332106438876</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>2.0750806076741224</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>2.0959355144943643</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2.1170000166126748</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>2.1382762204968184</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>2.1597662537849152</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>2.1814722654982011</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>2.2033964262559369</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2.2255409284924679</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2.2479079866764717</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.2704998375324057</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2.2933187402641826</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2.3163669767810915</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.3396468519259908</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.3631606937057947</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2.3869108535242765</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2.4108997064172097</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2.4351296512898744</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2.4596031111569499</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2.4843225333848165</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2.5092903899362979</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2.534509177617855</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>2.5599814183292713</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>2.585709659315846</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.6116964734231178</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.6379444593541526</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>2.6644562419294169</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>2.6912344723492621</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2.7182818284590451</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>2.7456010150169163</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.7731947639642978</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>2.8010658346990791</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>2.8292170143515598</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.8576511180631639</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2.8863709892679585</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2.9153794999769969</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2.9446795510655241</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>2.9742740725630656</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.0041660239464334</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3.0343583944356758</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.0648542032930024</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3.0956565001247109</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3.1267683651861553</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>3.1581929096897672</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>3.1899332761161845</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.2219926385284996</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3.2543742028896707</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3.2870812073831179</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>3.3201169227365472</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3.3534846525490236</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>3.3871877336213347</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>3.4212295362896734</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>3.4556134647626755</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>3.4903429574618414</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>3.5254214873653824</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>3.5608525623555205</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>3.5966397255692817</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>3.6327865557528094</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3.6692966676192444</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>3.706173712210199</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>3.7434213772608627</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>3.781043387568781</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>3.8190435053663361</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>3.8574255306969745</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>3.8961933017952148</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>3.9353506954704733</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>3.9749016274947477</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>4.0148500529942011</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>4.0551999668446745</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>4.0959554040711756</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>4.1371204402513921</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>4.1786991919232461</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>4.2206958169965523</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.2631145151688168</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4.3059595283452063</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4.3492351410627412</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>4.392945680918757</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>4.4370955190036643</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4.4816890703380645</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4.5267307943142523</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>4.5722251951421589</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>4.6181768222997812</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>4.6645902709881257</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>4.7114701825907419</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4.7588212451378542</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>4.8066481937751782</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>4.854955811237434</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>4.9037489283266229</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>4.9530324243951149</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>5.0028112278335879</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>5.0530903165638676</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>5.1038747185367255</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>5.1551695122346803</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>5.2069798271798486</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>5.2593108444468983</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>5.3121677971811669</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>5.3655559711219745</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>5.4194807051312059</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>5.4739473917271999</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>5.5289614776240041</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>5.5845284642760538</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>5.6406539084283205</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>5.6973434226719908</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>5.7546026760057307</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>5.8124373944025889</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>5.8708533613826015</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>5.9298564185911458</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>5.9894524663831135</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>6.0496474644129465</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>6.1104474322306102</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>6.1718584498835538</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>6.2338866585247175</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>6.2965382610266571</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>6.3598195226018319</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>6.4237367714291347</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>6.4882963992867122</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>6.553504862191148</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>6.6193686810430767</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>6.6858944422792685</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>6.7530887985312864</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>6.8209584692907494</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>6.8895102415812923</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>6.9587509706372721</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>7.0286875805892928</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>7.0993270651566327</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>7.1706764883466132</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>7.2427429851610121</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>7.3155337623095669</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>7.3890560989306504</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>7.4633173473191929</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>7.5383249336619222</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>7.6140863587799732</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>7.690609198878998</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>7.7679011063067707</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>7.845969810318449</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>7.9248231178494866</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>8.0044689142963534</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>8.084915164305059</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>8.1661699125676517</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>8.2482412846266602</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>8.3311374876876929</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>8.4148668114401293</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>8.499437628886124</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>8.5848583971778929</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>8.6711376584634561</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>8.7582840407408344</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>8.8463062587208832</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>8.9352131146987475</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>9.025013499434122</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>9.1157163930403051</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>9.2073308658822519</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>9.2998660794835857</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>9.3933312874427841</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9.4877358363585262</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>9.5830891667643758</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>9.6794008140728405</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>9.7766804095289039</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>9.8749376811731828</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>9.9741824548147182</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>10.074424655013587</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>10.175674306073333</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>10.277941533043448</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>10.381236562731843</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>10.485569724727576</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>10.59095145243378</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>10.697392284111054</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>10.804902863931257</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>10.913493943041976</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>11.023176380641601</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>11.133961145065307</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>11.245859314881844</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>11.358882080001457</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>11.473040742794833</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>11.588346719223392</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>11.704811539980854</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>11.822446851646363</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>11.941264417849103</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>12.06127612044472</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>12.182493960703473</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>12.30493006051041</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>12.428596663577544</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>12.553506136668229</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>12.679670970833877</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>12.807103782663029</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>12.935817315543076</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>13.065824440934556</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>13.197138159658358</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>13.329771603195772</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>13.463738035001692</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>13.599050851830924</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>13.735723585077926</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>13.873769902129904</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>14.013203607733615</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>14.154038645375801</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>14.296289098677603</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>14.439969192802881</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>14.585093295880792</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>14.731675920442569</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>14.879731724872837</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>15.029275514875401</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>15.180322244953899</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>15.332887019907195</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>15.486985096339938</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>15.642631884188171</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>15.799842948260395</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>15.958634009794029</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>16.119020948027543</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>16.281019801788428</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>16.444646771097048</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>16.609918218786699</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>16.776850672139872</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>16.945460824541019</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>17.115765537145876</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>17.287781840567639</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>17.46152693657999</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>17.637018199837321</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>17.814273179612197</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>17.993309601550319</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>18.17414536944306</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>18.356798567017925</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>18.541287459746869</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>18.727630496672919</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>18.915846312255038</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>19.105953728231651</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>19.297971755502758</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>19.491919596031121</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>19.6878166447624</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>19.885682491564729</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>20.085536923187668</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>20.287399925240926</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>20.491291684192941</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>20.6972325893895</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>20.905243235092758</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>21.115344422540609</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>21.327557162026903</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>21.541902675002412</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>21.758402396197081</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>21.977077975763418</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>22.197951281441636</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>22.421044400746343</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>22.646379643175397</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>22.873979542440807</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>23.103866858722185</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>23.336064580942711</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>23.570595929068126</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>23.80748435642867</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>24.046753552064498</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>24.288427443094555</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>24.532530197109352</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>24.779086224587694</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>25.028120181337815</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>25.279656970962893</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>25.533721747351528</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>25.790339917193062</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>26.049537142518336</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>26.311339343265892</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>26.575772699873955</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>26.842863655898565</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>27.112638920657883</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>27.385125471903219</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>27.660350558516747</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>27.938341703236507</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>28.219126705408609</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>28.502733643767282</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>28.789190879242675</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>29.078527057797078</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>29.370771113289432</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>29.665952270368855</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>29.964100047397011</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>30.265244259400085</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>30.569415021050208</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>30.876642749677046</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>31.186958168309459</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>31.500392308747937</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>31.81697651466769</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>32.13674244475316</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>32.459722075863795</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>32.785947706231894</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>33.115451958692312</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>33.448267783944907</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>33.784428463849558</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>34.123967614754356</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>34.466919190857389</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>34.813317487602014</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>35.163197145106615</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>35.51659315162847</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>35.873540847062763</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>36.234075926476464</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>36.598234443677988</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>36.966052814822504</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>37.337567822053657</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>37.712816617181744</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>38.09183672539902</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>38.474666049032123</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>38.861342871332468</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>39.251905860304497</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>39.646394072572605</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>40.044846957286715</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-860F-4D85-8244-07E709AAAFCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>A</c:v>
           </c:tx>
@@ -2289,6 +3426,58 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
@@ -3006,10 +4195,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
@@ -3042,16 +4231,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3066,7 +4255,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7536180" y="3337560"/>
+          <a:off x="7109460" y="3002280"/>
           <a:ext cx="457200" cy="373380"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3107,15 +4296,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>64770</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3130,8 +4319,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8496300" y="2971800"/>
-          <a:ext cx="457200" cy="373380"/>
+          <a:off x="8141970" y="2654300"/>
+          <a:ext cx="457200" cy="375920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3170,16 +4359,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>290830</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>138430</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>90170</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3194,8 +4383,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7978140" y="3703320"/>
-          <a:ext cx="457200" cy="373380"/>
+          <a:off x="7606030" y="3581400"/>
+          <a:ext cx="457200" cy="375920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3235,15 +4424,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>303530</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>73660</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3258,8 +4447,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8823960" y="3688080"/>
-          <a:ext cx="655320" cy="373380"/>
+          <a:off x="8837930" y="3572510"/>
+          <a:ext cx="655320" cy="375920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3308,12 +4497,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.59944</cdr:x>
-      <cdr:y>0.49907</cdr:y>
+      <cdr:x>0.56137</cdr:x>
+      <cdr:y>0.47625</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.79167</cdr:x>
-      <cdr:y>0.63519</cdr:y>
+      <cdr:x>0.7536</cdr:x>
+      <cdr:y>0.61237</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -3328,8 +4517,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2740660" y="1369060"/>
-          <a:ext cx="878840" cy="373380"/>
+          <a:off x="3426395" y="1816342"/>
+          <a:ext cx="1173298" cy="519136"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3460,6 +4649,102 @@
         </a:p>
       </cdr:txBody>
     </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.73575</cdr:x>
+      <cdr:y>0.61658</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.73749</cdr:x>
+      <cdr:y>0.92607</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBE3211D-2960-44F9-A3BA-4F2D88DA36D9}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1">
+          <a:off x="4490720" y="2351508"/>
+          <a:ext cx="10643" cy="1180362"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.97607</cdr:x>
+      <cdr:y>0.13187</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.97607</cdr:x>
+      <cdr:y>0.91941</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C5A8223-AD65-4C44-AA72-91336845CCA9}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="5957570" y="502920"/>
+          <a:ext cx="0" cy="3003550"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
   </cdr:relSizeAnchor>
 </c:userShapes>
 </file>
@@ -3763,8 +5048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9937A4F-C7BC-47E7-B5C9-D13F431183EE}">
   <dimension ref="A1:B401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7379,6 +8664,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>